<commit_message>
fixed issue with clean CPP datset
</commit_message>
<xml_diff>
--- a/All Data - CPP.xlsx
+++ b/All Data - CPP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="615" firstSheet="16" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="615" firstSheet="16" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Front page - notes on data" sheetId="1" r:id="rId1"/>
@@ -534,9 +534,6 @@
     <t>CO2 Emissions_Imputed_2004/05</t>
   </si>
   <si>
-    <t>CO2 Emissions_CO2 Emissions_Raw data_2005/06</t>
-  </si>
-  <si>
     <t>Child Poverty Rate_Raw data_2009</t>
   </si>
   <si>
@@ -939,12 +936,6 @@
     <t>Emergency Admissions Rate_Raw data_ 2012</t>
   </si>
   <si>
-    <t>Emergency Admissions Rate_Imputed_ data 2013</t>
-  </si>
-  <si>
-    <t>Emergency Admissions Rate_Imputed_ data 2014</t>
-  </si>
-  <si>
     <t>Emergency Admissions Rate_Projected_ 2015</t>
   </si>
   <si>
@@ -1006,6 +997,15 @@
   </si>
   <si>
     <t>Emergency Admissions Rate_Projected_ 2018/19-2020/21</t>
+  </si>
+  <si>
+    <t>CO2 Emissions_Raw data_2005/06</t>
+  </si>
+  <si>
+    <t>Emergency Admissions Rate_Imputed_ 2013</t>
+  </si>
+  <si>
+    <t>Emergency Admissions Rate_Imputed_2014</t>
   </si>
 </sst>
 </file>
@@ -20057,13 +20057,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="9" t="s">
         <v>162</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>163</v>
+        <v>318</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>152</v>
@@ -21466,55 +21466,55 @@
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -23386,49 +23386,49 @@
     <row r="1" spans="1:16" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>195</v>
-      </c>
       <c r="I1" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>188</v>
-      </c>
       <c r="K1" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -25098,55 +25098,55 @@
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>211</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -27014,55 +27014,55 @@
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>229</v>
-      </c>
       <c r="M1" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>217</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -28930,49 +28930,49 @@
   <sheetData>
     <row r="1" spans="1:16" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>243</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -30634,109 +30634,109 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AI1" sqref="AI1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="AB1" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AC1" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AD1" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AE1" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AF1" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AG1" s="9" t="s">
         <v>317</v>
-      </c>
-      <c r="AE1" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="AF1" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="AG1" s="9" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -34090,46 +34090,46 @@
     <row r="1" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>258</v>
-      </c>
       <c r="I1" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>250</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -37103,7 +37103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
@@ -37111,55 +37111,55 @@
   <sheetData>
     <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>274</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -45823,43 +45823,43 @@
     <row r="1" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="23"/>
       <c r="B1" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>279</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>280</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>282</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>283</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>285</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="N1" s="23" t="s">
         <v>287</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sorted CPP clean data as LA names were missing
</commit_message>
<xml_diff>
--- a/All Data - CPP.xlsx
+++ b/All Data - CPP.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\connachan.cara\Documents\CommunityPlanningOutcomesProfiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub-my.sharepoint.com/personal/cara_connachan_improvementservice_org_uk/Documents/CPOP Shiny Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="39" documentId="80B0005A750D15F7FC65CA39B4AACDA030BEF89C" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{BC976891-8B6E-4CDE-9959-E495A3599ADF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="615" firstSheet="16" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="615" firstSheet="16" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Front page - notes on data" sheetId="1" r:id="rId1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="313">
   <si>
     <t>CPP data</t>
   </si>
@@ -202,30 +203,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Argyll &amp; Bute</t>
-  </si>
-  <si>
-    <t>Dumfries &amp; Galloway</t>
-  </si>
-  <si>
-    <t>Edinburgh</t>
-  </si>
-  <si>
-    <t>Glasgow</t>
-  </si>
-  <si>
-    <t>Orkney</t>
-  </si>
-  <si>
-    <t>Perth &amp; Kinross</t>
-  </si>
-  <si>
-    <t>Shetland</t>
-  </si>
-  <si>
-    <t>Na h-Eileanan Siar</t>
   </si>
   <si>
     <t>% Of Babies With A Healthy Birthweight_Raw data_2004/05</t>
@@ -1002,16 +979,16 @@
     <t>CO2 Emissions_Raw data_2005/06</t>
   </si>
   <si>
-    <t>Emergency Admissions Rate_Imputed_ 2013</t>
+    <t>Emergency Admissions Rate_Imputed_2013</t>
   </si>
   <si>
-    <t>Emergency Admissions Rate_Imputed_2014</t>
+    <t>Emergency Admissions Rate_Imputed_ 2014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
@@ -1019,7 +996,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1068,20 +1045,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1118,9 +1102,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1169,19 +1153,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1191,12 +1168,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Comma 3" xfId="3"/>
+    <cellStyle name="Comma 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1507,7 +1492,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1278"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1534,10 +1519,10 @@
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="s">
@@ -1551,26 +1536,26 @@
       </c>
     </row>
     <row r="5" spans="2:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="30" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="165" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
@@ -18152,25 +18137,28 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -18641,52 +18629,55 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="23"/>
       <c r="B1" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>143</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -20048,52 +20039,55 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="9" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -21455,66 +21449,69 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -23371,64 +23368,64 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="1" max="1" width="22.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="9" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -25087,66 +25084,69 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>203</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -27003,66 +27003,69 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>228</v>
-      </c>
       <c r="M1" s="9" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -28919,60 +28922,63 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>235</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -30631,112 +30637,115 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AI1" sqref="AI1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="M1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="AB1" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="AC1" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="AD1" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="AE1" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="AF1" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="AG1" s="9" t="s">
         <v>309</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="AA1" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="AB1" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="AC1" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="AD1" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="AE1" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="AF1" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="AG1" s="9" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -34078,58 +34087,61 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -35689,54 +35701,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>64</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -35864,7 +35879,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="B5" s="15">
         <v>86.776859504132233</v>
@@ -35946,7 +35961,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B7" s="15">
         <v>88.921933085501863</v>
@@ -36192,7 +36207,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="B13" s="15">
         <v>88.744186046511629</v>
@@ -36356,7 +36371,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B17" s="15">
         <v>87.610890180483324</v>
@@ -36643,7 +36658,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="B24" s="15">
         <v>88.202247191011239</v>
@@ -36684,7 +36699,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B25" s="15">
         <v>88.124488124488124</v>
@@ -36807,7 +36822,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B28" s="15">
         <v>89.237668161434982</v>
@@ -37011,88 +37026,88 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="29">
+      <c r="B33" s="26">
         <v>88.702516033547113</v>
       </c>
-      <c r="C33" s="29">
+      <c r="C33" s="26">
         <v>89.728395061728392</v>
       </c>
-      <c r="D33" s="29">
+      <c r="D33" s="26">
         <v>87.63567720622936</v>
       </c>
-      <c r="E33" s="29">
+      <c r="E33" s="26">
         <v>90.369694203560016</v>
       </c>
-      <c r="F33" s="29">
+      <c r="F33" s="26">
         <v>87.704918032786878</v>
       </c>
-      <c r="G33" s="29">
+      <c r="G33" s="26">
         <v>90.300829875518673</v>
       </c>
-      <c r="H33" s="29">
+      <c r="H33" s="26">
         <v>89.638932496075356</v>
       </c>
-      <c r="I33" s="29">
+      <c r="I33" s="26">
         <v>90.395778364116097</v>
       </c>
-      <c r="J33" s="29">
+      <c r="J33" s="26">
         <v>89.912758996728456</v>
       </c>
-      <c r="K33" s="29">
+      <c r="K33" s="26">
         <v>91.304347826086953</v>
       </c>
-      <c r="L33" s="29">
+      <c r="L33" s="26">
         <v>90.465631929046566</v>
       </c>
-      <c r="M33" s="29">
+      <c r="M33" s="26">
         <v>89.989293361884364</v>
       </c>
-      <c r="N33" s="28"/>
+      <c r="N33" s="25"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="31">
+      <c r="B34" s="28">
         <v>88.701857813287816</v>
       </c>
-      <c r="C34" s="31">
+      <c r="C34" s="28">
         <v>88.997593284677251</v>
       </c>
-      <c r="D34" s="31">
+      <c r="D34" s="28">
         <v>89.021610113608531</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="28">
         <v>89.265830036341498</v>
       </c>
-      <c r="F34" s="31">
+      <c r="F34" s="28">
         <v>89.193791574279373</v>
       </c>
-      <c r="G34" s="31">
+      <c r="G34" s="28">
         <v>89.429587151865945</v>
       </c>
-      <c r="H34" s="31">
+      <c r="H34" s="28">
         <v>89.639146584363615</v>
       </c>
-      <c r="I34" s="31">
+      <c r="I34" s="28">
         <v>89.353903094361115</v>
       </c>
-      <c r="J34" s="31">
+      <c r="J34" s="28">
         <v>89.524980727579745</v>
       </c>
-      <c r="K34" s="31">
+      <c r="K34" s="28">
         <v>89.963410241340739</v>
       </c>
-      <c r="L34" s="31">
+      <c r="L34" s="28">
         <v>89.953231212012199</v>
       </c>
-      <c r="M34" s="31">
+      <c r="M34" s="28">
         <v>90.080362583790375</v>
       </c>
-      <c r="N34" s="28"/>
+      <c r="N34" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37100,66 +37115,69 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>266</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -39016,52 +39034,55 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -40177,52 +40198,55 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -41584,52 +41608,55 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="L1" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="19" t="s">
         <v>100</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -42995,54 +43022,57 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -44404,52 +44434,55 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -45811,55 +45844,58 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="23"/>
       <c r="B1" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="N1" s="23" t="s">
         <v>279</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>280</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>282</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>285</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>286</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -47320,586 +47356,592 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" style="33" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="33"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25"/>
-      <c r="B1" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>136</v>
+      <c r="A1" s="32"/>
+      <c r="B1" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="35">
         <v>25.1685725</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="35">
         <v>24.544817500000001</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="35">
         <v>24.224468999999999</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="35">
         <v>24.1760643</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="35">
         <v>26.575287299999999</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="35">
         <v>26.056575899999999</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="35">
         <v>24.793096999999999</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="35">
         <v>24.5703827</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="35">
         <v>24.211532999999999</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="35">
         <v>24.428145000000001</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="35">
         <v>24.813198100000001</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="35">
         <v>24.389413699999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="27">
+      <c r="A5" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="35">
         <v>24.991161099999999</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="35">
         <v>24.6590308</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="35">
         <v>25.283632799999999</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="35">
         <v>25.1225664</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="35">
         <v>23.653530700000001</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="35">
         <v>23.631250099999999</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="35">
         <v>24.218609699999998</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="35">
         <v>24.176622500000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="27">
+      <c r="A7" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="35">
         <v>24.158192100000001</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="35">
         <v>25.265371200000001</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="35">
         <v>24.617848500000001</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="35">
         <v>23.753478099999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="35">
         <v>23.8479578</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="35">
         <v>23.5158062</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="35">
         <v>23.244762399999999</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="35">
         <v>24.366558099999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="35">
         <v>23.791586599999999</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="35">
         <v>23.045939099999998</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="35">
         <v>24.228767699999999</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="35">
         <v>23.4100474</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="35">
         <v>25.604061300000001</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="35">
         <v>24.476621900000001</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="35">
         <v>25.140613299999998</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="35">
         <v>24.8836066</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="35">
         <v>24.299972499999999</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="35">
         <v>24.046780500000001</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="35">
         <v>24.509022099999999</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="35">
         <v>25.212893699999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="35">
         <v>24.2614774</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="35">
         <v>25.316192900000001</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="35">
         <v>25.259052199999999</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="35">
         <v>24.7013195</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="35">
         <v>24.7924179</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="35">
         <v>24.1522048</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="35">
         <v>24.605514800000002</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="35">
         <v>24.5022038</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="27">
+      <c r="A14" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="35">
         <v>25.2134939</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="35">
         <v>24.066900100000002</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="35">
         <v>24.088752800000002</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="35">
         <v>24.895787800000001</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="35">
         <v>23.2544547</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="35">
         <v>24.411102899999999</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="35">
         <v>24.524531400000001</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="35">
         <v>24.7178124</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="35">
         <v>25.116999700000001</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="35">
         <v>24.046277799999999</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="35">
         <v>24.579057500000001</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="35">
         <v>24.5615515</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="35">
         <v>23.7573121</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="35">
         <v>23.4594463</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="35">
         <v>24.3107708</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="35">
         <v>23.7573075</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="35">
         <v>25.035947799999999</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="35">
         <v>24.629873199999999</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="35">
         <v>24.910717300000002</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="35">
         <v>24.206233600000001</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="35">
         <v>25.900677699999999</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="35">
         <v>24.344720200000001</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="35">
         <v>23.8970652</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="35">
         <v>24.671051500000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="35">
         <v>24.703280400000001</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="35">
         <v>24.2154417</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="35">
         <v>24.350711100000002</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="35">
         <v>25.693141499999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="35">
         <v>25.840653</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="35">
         <v>24.546849699999999</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="35">
         <v>24.6444829</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="35">
         <v>23.859061400000002</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="35">
         <v>27.196384900000002</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="35">
         <v>25.2857913</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="35">
         <v>24.951658900000002</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="35">
         <v>25.637066399999998</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="35">
         <v>23.9949464</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="35">
         <v>23.9103861</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="35">
         <v>24.7577912</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="35">
         <v>25.127268600000001</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="35">
         <v>25.852315000000001</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C24" s="35">
         <v>27.105867100000001</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="35">
         <v>26.560321299999998</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="35">
         <v>27.586240100000001</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="27">
+      <c r="A25" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="35">
         <v>24.592188499999999</v>
       </c>
-      <c r="C25" s="27">
+      <c r="C25" s="35">
         <v>24.230472299999999</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="35">
         <v>24.630752699999999</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="35">
         <v>24.3445252</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="27">
+      <c r="B26" s="35">
         <v>24.662311200000001</v>
       </c>
-      <c r="C26" s="27">
+      <c r="C26" s="35">
         <v>24.521911800000002</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="35">
         <v>24.595040600000001</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="35">
         <v>24.305073100000001</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="35">
         <v>24.839924400000001</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="35">
         <v>23.999415500000001</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="35">
         <v>24.2950892</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="35">
         <v>24.4405009</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="35">
         <v>26.2108797</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C28" s="35">
         <v>26.384240999999999</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="35">
         <v>25.5209008</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="35">
         <v>25.202959</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="35">
         <v>23.644127000000001</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C29" s="35">
         <v>23.832291300000001</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="35">
         <v>23.596812700000001</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="35">
         <v>23.8446958</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="35">
         <v>24.9534512</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C30" s="35">
         <v>24.4452076</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D30" s="35">
         <v>24.665150199999999</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="35">
         <v>24.303855800000001</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="27">
+      <c r="B31" s="35">
         <v>24.9559031</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C31" s="35">
         <v>25.3253138</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="35">
         <v>25.3317184</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E31" s="35">
         <v>24.226721099999999</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="35">
         <v>23.751834200000001</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C32" s="35">
         <v>24.104337900000001</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D32" s="35">
         <v>23.9779731</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="35">
         <v>24.105408000000001</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="27">
+      <c r="B33" s="35">
         <v>23.875482000000002</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C33" s="35">
         <v>23.813690399999999</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D33" s="35">
         <v>24.311253499999999</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="35">
         <v>24.3604162</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="33">
+      <c r="B34" s="37">
         <v>24.6609245</v>
       </c>
-      <c r="C34" s="33">
+      <c r="C34" s="37">
         <v>24.299565999999999</v>
       </c>
-      <c r="D34" s="33">
+      <c r="D34" s="37">
         <v>24.539170200000001</v>
       </c>
-      <c r="E34" s="33">
+      <c r="E34" s="37">
         <v>24.423405899999999</v>
       </c>
     </row>
@@ -47909,12 +47951,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="efa9a972-862c-4aae-ab3c-3d18e64e713d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -48107,17 +48148,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="efa9a972-862c-4aae-ab3c-3d18e64e713d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4724EAE4-ADED-4996-8793-973D115FDA12}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{051C8AFB-F743-46F1-B17F-4A3416CD730A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="9ed984fb-628d-48c7-84a0-112ec4a4bd9e"/>
+    <ds:schemaRef ds:uri="efa9a972-862c-4aae-ab3c-3d18e64e713d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -48142,18 +48193,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{051C8AFB-F743-46F1-B17F-4A3416CD730A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4724EAE4-ADED-4996-8793-973D115FDA12}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9ed984fb-628d-48c7-84a0-112ec4a4bd9e"/>
-    <ds:schemaRef ds:uri="efa9a972-862c-4aae-ab3c-3d18e64e713d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>